<commit_message>
update to orders object
</commit_message>
<xml_diff>
--- a/data-model.xlsx
+++ b/data-model.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Relationships" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="data-model" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="contacts" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="rides" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Journey" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="orders" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="77">
   <si>
     <t>Object1</t>
   </si>
@@ -44,7 +44,7 @@
 Comments</t>
   </si>
   <si>
-    <t>Rides</t>
+    <t>Journey</t>
   </si>
   <si>
     <t>Contact</t>
@@ -56,7 +56,7 @@
     <t>1-2-Many</t>
   </si>
   <si>
-    <t>A ride can have many contacts</t>
+    <t>A journey can have many contacts</t>
   </si>
   <si>
     <t>Orders</t>
@@ -68,6 +68,9 @@
     <t>In this case cannot have a master detail to Orders, cannot delete detail side that is a standard object</t>
   </si>
   <si>
+    <t>a contact can place 1 order</t>
+  </si>
+  <si>
     <t>Field Name </t>
   </si>
   <si>
@@ -179,7 +182,13 @@
     <t>Driver Name</t>
   </si>
   <si>
-    <t>Car Brand </t>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Max No: Passengers</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
   <si>
     <t>Day</t>
@@ -194,9 +203,6 @@
     <t>No: kilometres</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Price Per kilometre</t>
   </si>
   <si>
@@ -234,6 +240,12 @@
   </si>
   <si>
     <t>Biling street</t>
+  </si>
+  <si>
+    <t>address(lookup Contact)</t>
+  </si>
+  <si>
+    <t>map billing to mail address</t>
   </si>
   <si>
     <t>billing city</t>
@@ -398,7 +410,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,6 +509,14 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -516,10 +536,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -580,6 +600,23 @@
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +637,7 @@
   </sheetPr>
   <dimension ref="A1:A65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -647,7 +684,7 @@
   <dimension ref="1:19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -658,31 +695,31 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6428571428571"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3010204081633"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.515306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="67.9438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="53.8724489795918"/>
     <col collapsed="false" hidden="false" max="28" min="8" style="0" width="16.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -708,7 +745,7 @@
     </row>
     <row r="2" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -741,15 +778,15 @@
     </row>
     <row r="3" s="19" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
@@ -778,107 +815,107 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="E9" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -911,80 +948,80 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="20" t="n">
         <v>255</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="20" t="n">
         <v>40</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="D15" s="20" t="n">
         <v>80</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="20" t="n">
         <v>20</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="20" t="n">
         <v>80</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -1017,10 +1054,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1039,10 +1076,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1059,25 +1096,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1134,68 +1171,76 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1216,42 +1261,43 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6377551020408"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0765306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="7" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="27" min="8" style="0" width="16.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1277,7 +1323,7 @@
     </row>
     <row r="2" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1310,66 +1356,96 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>